<commit_message>
Finished IMDb matching, now doing Metacritic matching
</commit_message>
<xml_diff>
--- a/data_2017_5_9/imdb/imdbduplicates.xlsx
+++ b/data_2017_5_9/imdb/imdbduplicates.xlsx
@@ -382,13 +382,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM2"/>
+  <dimension ref="A1:AP2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:39" s="0" outlineLevel="0">
+    <row r="1" spans="1:42" s="0" outlineLevel="0">
       <c r="A1" t="inlineStr">
         <is>
           <t>key</t>
@@ -580,6 +580,21 @@
         </is>
       </c>
       <c r="AM1" t="inlineStr">
+        <is>
+          <t>V39</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>V40</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>V41</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
         <is>
           <t>MatchSequence</t>
         </is>

</xml_diff>